<commit_message>
Exámenes Ordinario/Extraordinario 30 mayo de 2024 - Lap HP
Se actualiza el repositorio con los exámenes ordinario y extraordinario de Física III.
</commit_message>
<xml_diff>
--- a/Bitacoras/NRC_124_Grupo_43/Concentrado_Grupo_43.xlsx
+++ b/Bitacoras/NRC_124_Grupo_43/Concentrado_Grupo_43.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusto\OneDrive\Documentos\Cursos_UVM\Plan PU\Fisica_3\Bitacoras\NRC_124_Grupo_43\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D90C48-0D39-471B-87B0-3E2FAF722272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{056EA472-30B4-4DB2-8E28-763DE14D2DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A7110BCD-1518-461B-A6CF-DE815350E466}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" xr2:uid="{A7110BCD-1518-461B-A6CF-DE815350E466}"/>
   </bookViews>
   <sheets>
     <sheet name="Concentrado" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Concentrado!$A$2:$Y$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Concentrado!$A$2:$AA$28</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="46">
   <si>
     <t>Alumno</t>
   </si>
@@ -171,6 +172,12 @@
   </si>
   <si>
     <t>Porcentaje</t>
+  </si>
+  <si>
+    <t>Ordinario</t>
+  </si>
+  <si>
+    <t>Segunda Vuelta</t>
   </si>
 </sst>
 </file>
@@ -477,7 +484,227 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="25">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -845,11 +1072,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F1F25DF-27B5-442B-9AFD-7505FCE4FC7E}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:AC28"/>
+  <dimension ref="A1:AE28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="4785" ySplit="1035" topLeftCell="Q7" activePane="bottomRight"/>
+      <selection activeCell="A2" sqref="A2"/>
+      <selection pane="topRight" activeCell="X1" sqref="X1"/>
+      <selection pane="bottomLeft" activeCell="V3" sqref="V3"/>
+      <selection pane="bottomRight" activeCell="AA12" sqref="AA12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -879,12 +1109,14 @@
     <col min="23" max="23" width="8.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="6.28515625" customWidth="1"/>
-    <col min="29" max="29" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.28515625" customWidth="1"/>
+    <col min="31" max="31" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B1" s="36" t="s">
         <v>31</v>
       </c>
@@ -914,7 +1146,7 @@
       <c r="T1" s="46"/>
       <c r="U1" s="47"/>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -990,8 +1222,15 @@
       <c r="Y2" s="2" t="s">
         <v>37</v>
       </c>
+      <c r="Z2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB2" s="2"/>
     </row>
-    <row r="3" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1076,7 +1315,7 @@
         <v>Extraordinario</v>
       </c>
     </row>
-    <row r="4" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1161,7 +1400,7 @@
         <v>Exento</v>
       </c>
     </row>
-    <row r="5" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1245,8 +1484,15 @@
         <f t="shared" si="7"/>
         <v>Primera Vuelta</v>
       </c>
+      <c r="Z5" s="2">
+        <v>7.21</v>
+      </c>
+      <c r="AA5" s="29">
+        <f t="shared" ref="AA5:AA6" si="8">(X5+Z5)/2</f>
+        <v>6.8467137096774184</v>
+      </c>
     </row>
-    <row r="6" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1330,17 +1576,24 @@
         <f t="shared" si="7"/>
         <v>Primera Vuelta</v>
       </c>
-      <c r="AA6" s="1" t="s">
+      <c r="Z6" s="2">
+        <v>4.28</v>
+      </c>
+      <c r="AA6" s="29">
+        <f t="shared" si="8"/>
+        <v>4.7774536290322587</v>
+      </c>
+      <c r="AC6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AB6" s="1" t="s">
+      <c r="AD6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AC6" s="1" t="s">
+      <c r="AE6" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1424,19 +1677,19 @@
         <f t="shared" si="7"/>
         <v>Exento</v>
       </c>
-      <c r="AA7" t="s">
+      <c r="AC7" t="s">
         <v>39</v>
       </c>
-      <c r="AB7" s="2">
+      <c r="AD7" s="2">
         <f>COUNTIF(Y3:Y28,"=Extraordinario")</f>
         <v>3</v>
       </c>
-      <c r="AC7" s="28">
-        <f>AB7/26</f>
+      <c r="AE7" s="28">
+        <f>AD7/26</f>
         <v>0.11538461538461539</v>
       </c>
     </row>
-    <row r="8" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1520,19 +1773,26 @@
         <f t="shared" si="7"/>
         <v>Primera Vuelta</v>
       </c>
-      <c r="AA8" t="s">
+      <c r="Z8" s="2">
+        <v>5.93</v>
+      </c>
+      <c r="AA8" s="29">
+        <f>(X8+Z8)/2</f>
+        <v>5.674764112903226</v>
+      </c>
+      <c r="AC8" t="s">
         <v>40</v>
       </c>
-      <c r="AB8" s="2">
+      <c r="AD8" s="2">
         <f>COUNTIF(Y3:Y28,"=Primera Vuelta")</f>
         <v>13</v>
       </c>
-      <c r="AC8" s="28">
-        <f t="shared" ref="AC8:AC9" si="8">AB8/26</f>
+      <c r="AE8" s="28">
+        <f t="shared" ref="AE8:AE9" si="9">AD8/26</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1616,19 +1876,19 @@
         <f t="shared" si="7"/>
         <v>Exento</v>
       </c>
-      <c r="AA9" t="s">
+      <c r="AC9" t="s">
         <v>41</v>
       </c>
-      <c r="AB9" s="2">
+      <c r="AD9" s="2">
         <f>COUNTIF(Y3:Y28,"=Exento")</f>
         <v>10</v>
       </c>
-      <c r="AC9" s="28">
-        <f t="shared" si="8"/>
+      <c r="AE9" s="28">
+        <f t="shared" si="9"/>
         <v>0.38461538461538464</v>
       </c>
     </row>
-    <row r="10" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1713,7 +1973,7 @@
         <v>Exento</v>
       </c>
     </row>
-    <row r="11" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1798,7 +2058,7 @@
         <v>Extraordinario</v>
       </c>
     </row>
-    <row r="12" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1882,8 +2142,21 @@
         <f t="shared" si="7"/>
         <v>Primera Vuelta</v>
       </c>
+      <c r="Z12" s="2">
+        <v>5.35</v>
+      </c>
+      <c r="AA12" s="29">
+        <f>(X12+Z12)/2</f>
+        <v>5.8172499999999996</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD12" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="13" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1967,8 +2240,15 @@
         <f t="shared" si="7"/>
         <v>Extraordinario</v>
       </c>
+      <c r="Z13" s="2">
+        <v>8.84</v>
+      </c>
+      <c r="AA13" s="29">
+        <f t="shared" ref="AA13:AA18" si="10">(X13+Z13)/2</f>
+        <v>6.2123749999999998</v>
+      </c>
     </row>
-    <row r="14" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -2053,7 +2333,7 @@
         <v>Exento</v>
       </c>
     </row>
-    <row r="15" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -2137,8 +2417,15 @@
         <f t="shared" si="7"/>
         <v>Primera Vuelta</v>
       </c>
+      <c r="Z15" s="2">
+        <v>5.97</v>
+      </c>
+      <c r="AA15" s="29">
+        <f t="shared" si="10"/>
+        <v>5.5435383064516124</v>
+      </c>
     </row>
-    <row r="16" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -2222,8 +2509,15 @@
         <f t="shared" si="7"/>
         <v>Primera Vuelta</v>
       </c>
+      <c r="Z16" s="2">
+        <v>8.6</v>
+      </c>
+      <c r="AA16" s="29">
+        <f t="shared" si="10"/>
+        <v>7.0911088709677417</v>
+      </c>
     </row>
-    <row r="17" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -2307,8 +2601,15 @@
         <f t="shared" si="7"/>
         <v>Primera Vuelta</v>
       </c>
+      <c r="Z17" s="2">
+        <v>7.21</v>
+      </c>
+      <c r="AA17" s="29">
+        <f t="shared" si="10"/>
+        <v>7.4030987903225807</v>
+      </c>
     </row>
-    <row r="18" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -2392,8 +2693,15 @@
         <f t="shared" si="7"/>
         <v>Primera Vuelta</v>
       </c>
+      <c r="Z18" s="2">
+        <v>6.84</v>
+      </c>
+      <c r="AA18" s="29">
+        <f t="shared" si="10"/>
+        <v>6.0220685483870966</v>
+      </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -2477,8 +2785,15 @@
         <f t="shared" si="7"/>
         <v>Primera Vuelta</v>
       </c>
+      <c r="Z19" s="2">
+        <v>6.98</v>
+      </c>
+      <c r="AA19" s="29">
+        <f>(X19+Z19)/2</f>
+        <v>6.1934540322580647</v>
+      </c>
     </row>
-    <row r="20" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -2563,7 +2878,7 @@
         <v>Exento</v>
       </c>
     </row>
-    <row r="21" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -2647,8 +2962,15 @@
         <f t="shared" si="7"/>
         <v>Primera Vuelta</v>
       </c>
+      <c r="Z21" s="2">
+        <v>7.45</v>
+      </c>
+      <c r="AA21" s="29">
+        <f t="shared" ref="AA21:AA22" si="11">(X21+Z21)/2</f>
+        <v>7.1687963709677422</v>
+      </c>
     </row>
-    <row r="22" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -2732,8 +3054,15 @@
         <f t="shared" si="7"/>
         <v>Primera Vuelta</v>
       </c>
+      <c r="Z22" s="2">
+        <v>4.46</v>
+      </c>
+      <c r="AA22" s="29">
+        <f t="shared" si="11"/>
+        <v>5.6342157258064516</v>
+      </c>
     </row>
-    <row r="23" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -2818,7 +3147,7 @@
         <v>Exento</v>
       </c>
     </row>
-    <row r="24" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -2903,7 +3232,7 @@
         <v>Exento</v>
       </c>
     </row>
-    <row r="25" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>11</v>
       </c>
@@ -2987,8 +3316,15 @@
         <f t="shared" si="7"/>
         <v>Primera Vuelta</v>
       </c>
+      <c r="Z25" s="2">
+        <v>7.44</v>
+      </c>
+      <c r="AA25" s="29">
+        <f t="shared" ref="AA25:AA26" si="12">(X25+Z25)/2</f>
+        <v>7.6068669354838701</v>
+      </c>
     </row>
-    <row r="26" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>12</v>
       </c>
@@ -3072,8 +3408,15 @@
         <f t="shared" si="7"/>
         <v>Primera Vuelta</v>
       </c>
+      <c r="Z26" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA26" s="29">
+        <f t="shared" si="12"/>
+        <v>2.9661290322580651</v>
+      </c>
     </row>
-    <row r="27" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -3158,7 +3501,7 @@
         <v>Exento</v>
       </c>
     </row>
-    <row r="28" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -3244,13 +3587,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:Y28" xr:uid="{1F1F25DF-27B5-442B-9AFD-7505FCE4FC7E}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="González Talavera Axel Izachard"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:A28">
     <sortCondition ref="A3:A28"/>
   </sortState>
@@ -3260,17 +3596,39 @@
     <mergeCell ref="L1:P1"/>
     <mergeCell ref="Q1:U1"/>
   </mergeCells>
-  <conditionalFormatting sqref="Y3:Y28">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Extraordinario">
+  <conditionalFormatting sqref="Y3:Z28">
+    <cfRule type="containsText" dxfId="24" priority="3" operator="containsText" text="Extraordinario">
       <formula>NOT(ISERROR(SEARCH("Extraordinario",Y3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Primera Vuelta">
+    <cfRule type="containsText" dxfId="23" priority="4" operator="containsText" text="Primera Vuelta">
       <formula>NOT(ISERROR(SEARCH("Primera Vuelta",Y3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Exento">
+    <cfRule type="containsText" dxfId="22" priority="5" operator="containsText" text="Exento">
       <formula>NOT(ISERROR(SEARCH("Exento",Y3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA5:AA6 AA8 AA12:AA13 AA15:AA19 AA21:AA22 AA25:AA26">
+    <cfRule type="cellIs" dxfId="21" priority="2" operator="greaterThan">
+      <formula>5.9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA6 AA8 AA12:AA13 AA15:AA19 AA25:AA26 AA21:AA22">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="lessThan">
+      <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC917799-CDE1-4864-B452-D3438F97037B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Actualización 25 de junio de 2024 - Lap HP
Se actualiza con las evaluaciones finales del curso.
</commit_message>
<xml_diff>
--- a/Bitacoras/NRC_124_Grupo_43/Concentrado_Grupo_43.xlsx
+++ b/Bitacoras/NRC_124_Grupo_43/Concentrado_Grupo_43.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusto\OneDrive\Documentos\Cursos_UVM\Plan PU\Fisica_3\Bitacoras\NRC_124_Grupo_43\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{056EA472-30B4-4DB2-8E28-763DE14D2DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C24A157-935E-49AF-98C2-CB5AF207083E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" xr2:uid="{A7110BCD-1518-461B-A6CF-DE815350E466}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A7110BCD-1518-461B-A6CF-DE815350E466}"/>
   </bookViews>
   <sheets>
     <sheet name="Concentrado" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
   <si>
     <t>Alumno</t>
   </si>
@@ -484,207 +484,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="25">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1079,7 +879,7 @@
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="X1" sqref="X1"/>
       <selection pane="bottomLeft" activeCell="V3" sqref="V3"/>
-      <selection pane="bottomRight" activeCell="AA12" sqref="AA12"/>
+      <selection pane="bottomRight" activeCell="Y14" sqref="Y14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1682,11 +1482,11 @@
       </c>
       <c r="AD7" s="2">
         <f>COUNTIF(Y3:Y28,"=Extraordinario")</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AE7" s="28">
         <f>AD7/26</f>
-        <v>0.11538461538461539</v>
+        <v>7.6923076923076927E-2</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
@@ -1785,11 +1585,11 @@
       </c>
       <c r="AD8" s="2">
         <f>COUNTIF(Y3:Y28,"=Primera Vuelta")</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AE8" s="28">
         <f t="shared" ref="AE8:AE9" si="9">AD8/26</f>
-        <v>0.5</v>
+        <v>0.53846153846153844</v>
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
@@ -2236,9 +2036,8 @@
         <f t="shared" si="6"/>
         <v>3.5847499999999997</v>
       </c>
-      <c r="Y13" t="str">
-        <f t="shared" si="7"/>
-        <v>Extraordinario</v>
+      <c r="Y13" t="s">
+        <v>40</v>
       </c>
       <c r="Z13" s="2">
         <v>8.84</v>
@@ -3597,23 +3396,23 @@
     <mergeCell ref="Q1:U1"/>
   </mergeCells>
   <conditionalFormatting sqref="Y3:Z28">
-    <cfRule type="containsText" dxfId="24" priority="3" operator="containsText" text="Extraordinario">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="Extraordinario">
       <formula>NOT(ISERROR(SEARCH("Extraordinario",Y3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="4" operator="containsText" text="Primera Vuelta">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="Primera Vuelta">
       <formula>NOT(ISERROR(SEARCH("Primera Vuelta",Y3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="5" operator="containsText" text="Exento">
+    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="Exento">
       <formula>NOT(ISERROR(SEARCH("Exento",Y3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA5:AA6 AA8 AA12:AA13 AA15:AA19 AA21:AA22 AA25:AA26">
-    <cfRule type="cellIs" dxfId="21" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>5.9</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA6 AA8 AA12:AA13 AA15:AA19 AA25:AA26 AA21:AA22">
-    <cfRule type="cellIs" dxfId="20" priority="1" operator="lessThan">
+  <conditionalFormatting sqref="AA6 AA8 AA12:AA13 AA15:AA19 AA21:AA22 AA25:AA26">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>